<commit_message>
Final edit for the database sample
</commit_message>
<xml_diff>
--- a/inventory_sample_data.xlsx
+++ b/inventory_sample_data.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Earth\git\arnonnut_inventory\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091FCC23-0B34-4E5A-A8CC-D66C2B5A925E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="suppliers" sheetId="1" r:id="rId1"/>
@@ -14,12 +20,12 @@
     <sheet name="stock_levels" sheetId="5" r:id="rId5"/>
     <sheet name="users" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="117">
   <si>
     <t>supplier_id</t>
   </si>
@@ -375,8 +381,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -428,9 +434,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -439,13 +448,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -483,7 +500,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -517,6 +534,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -551,9 +569,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -726,14 +745,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -744,7 +763,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>101</v>
       </c>
@@ -755,7 +774,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>102</v>
       </c>
@@ -766,7 +785,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>103</v>
       </c>
@@ -783,14 +802,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -804,7 +823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -818,7 +837,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -832,7 +851,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -846,7 +865,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -860,7 +879,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -874,7 +893,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -888,7 +907,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -902,7 +921,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -916,7 +935,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -930,7 +949,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -944,7 +963,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -958,7 +977,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -972,7 +991,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -992,14 +1011,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -1010,7 +1029,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>501</v>
       </c>
@@ -1021,7 +1040,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>502</v>
       </c>
@@ -1032,7 +1051,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>503</v>
       </c>
@@ -1049,14 +1068,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -1070,7 +1089,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -1084,7 +1103,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -1098,7 +1117,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -1112,7 +1131,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -1126,7 +1145,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -1140,7 +1159,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -1154,7 +1173,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -1168,7 +1187,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>57</v>
       </c>
@@ -1182,7 +1201,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>58</v>
       </c>
@@ -1196,7 +1215,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>59</v>
       </c>
@@ -1210,7 +1229,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -1224,7 +1243,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -1238,7 +1257,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -1252,7 +1271,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>63</v>
       </c>
@@ -1272,14 +1291,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1290,7 +1309,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1301,7 +1320,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1312,7 +1331,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1323,7 +1342,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1334,7 +1353,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1345,7 +1364,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1356,7 +1375,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1367,7 +1386,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1378,7 +1397,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1389,7 +1408,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1400,7 +1419,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1411,7 +1430,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1422,7 +1441,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1433,7 +1452,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1450,14 +1469,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="8" max="8" width="22.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>68</v>
       </c>
@@ -1479,8 +1503,11 @@
       <c r="G1" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>201</v>
       </c>
@@ -1502,8 +1529,11 @@
       <c r="G2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>202</v>
       </c>
@@ -1525,8 +1555,11 @@
       <c r="G3" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>203</v>
       </c>
@@ -1548,8 +1581,11 @@
       <c r="G4" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>204</v>
       </c>
@@ -1571,8 +1607,11 @@
       <c r="G5" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>205</v>
       </c>
@@ -1594,8 +1633,11 @@
       <c r="G6" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>206</v>
       </c>
@@ -1617,8 +1659,11 @@
       <c r="G7" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>207</v>
       </c>
@@ -1640,8 +1685,11 @@
       <c r="G8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>208</v>
       </c>
@@ -1663,8 +1711,11 @@
       <c r="G9" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="H9">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>209</v>
       </c>
@@ -1685,6 +1736,9 @@
       </c>
       <c r="G10" t="s">
         <v>104</v>
+      </c>
+      <c r="H10">
+        <v>501</v>
       </c>
     </row>
   </sheetData>

</xml_diff>